<commit_message>
Creating the queue item and assets
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andreea.ghetu\Documents\UiPath\CSharpChanges\StudioTemplates\REFramework\C#\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/jose_ordonez_uipath_com/Documents/Documents/UiPath/2024/Fantastic Build and Grow/Automations/Filling_Dispatcher_JO/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96902286-4E3C-425E-A0BF-F83C72A8C5F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{96902286-4E3C-425E-A0BF-F83C72A8C5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AA9E8B0-A408-4BDC-8882-0933B52433C0}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="18000" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6750" yWindow="3015" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -85,13 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -161,6 +154,24 @@
   </si>
   <si>
     <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>Jose Ordonez</t>
+  </si>
+  <si>
+    <t>Filling Analyzer URL</t>
+  </si>
+  <si>
+    <t>Filing_URLName</t>
+  </si>
+  <si>
+    <t>Filing_URL</t>
+  </si>
+  <si>
+    <t>Filing_Dispatcher_JO</t>
+  </si>
+  <si>
+    <t>Filings</t>
   </si>
 </sst>
 </file>
@@ -212,21 +223,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -245,9 +251,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -285,7 +291,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -391,7 +397,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -533,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -544,7 +550,7 @@
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -591,35 +597,35 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
-      <c r="A3" s="7" t="s">
-        <v>38</v>
+      <c r="A3" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="7"/>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -687,24 +693,22 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
-      <c r="A3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="5">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>33</v>
+      <c r="C3" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
@@ -725,7 +729,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -747,7 +751,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -758,7 +762,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -769,56 +773,51 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B15">
         <v>2</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
-      <c r="A15" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="5">
-        <v>2</v>
-      </c>
-      <c r="C15" s="5" t="s">
+    <row r="17" spans="1:3" ht="45">
+      <c r="A17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="45">
-      <c r="A17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="5" t="b">
+      <c r="B17" t="b">
         <v>0</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>40</v>
+      <c r="C17" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -832,7 +831,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -851,7 +850,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -879,7 +878,20 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Filing_Dispatcher_JO: Process tested in attended mode and finallyit was published in Jose Ordonez folder.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/jose_ordonez_uipath_com/Documents/Documents/UiPath/2024/Fantastic Build and Grow/Automations/Filling_Dispatcher_JO/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/jose_ordonez_uipath_com/Documents/Documents/UiPath/2024/Fantastic Build and Grow/Automations/Filing_Dispatcher_JO/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{96902286-4E3C-425E-A0BF-F83C72A8C5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AA9E8B0-A408-4BDC-8882-0933B52433C0}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{96902286-4E3C-425E-A0BF-F83C72A8C5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A780AB67-C910-4298-84D2-2351361CBA31}"/>
   <bookViews>
-    <workbookView xWindow="6750" yWindow="3015" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11925" yWindow="3930" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -95,83 +95,82 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>Jose Ordonez</t>
+  </si>
+  <si>
+    <t>Filling Analyzer URL</t>
+  </si>
+  <si>
+    <t>Filing_URLName</t>
+  </si>
+  <si>
+    <t>Filing_URL</t>
+  </si>
+  <si>
+    <t>Filing_Dispatcher_JO</t>
+  </si>
+  <si>
+    <t>Filings</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>Jose Ordonez</t>
-  </si>
-  <si>
-    <t>Filling Analyzer URL</t>
-  </si>
-  <si>
-    <t>Filing_URLName</t>
-  </si>
-  <si>
-    <t>Filing_URL</t>
-  </si>
-  <si>
-    <t>Filing_Dispatcher_JO</t>
-  </si>
-  <si>
-    <t>Filings</t>
   </si>
 </sst>
 </file>
@@ -248,6 +247,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -550,7 +553,7 @@
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -597,10 +600,10 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -608,10 +611,13 @@
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -622,7 +628,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -693,18 +699,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -729,7 +735,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -751,7 +757,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -762,7 +768,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -773,51 +779,51 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
         <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -850,7 +856,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -880,16 +886,16 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
       <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
         <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>